<commit_message>
auto assign,auto update & delete order integrated
</commit_message>
<xml_diff>
--- a/UserReport.xlsx
+++ b/UserReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -28,6 +28,15 @@
     <t>Role</t>
   </si>
   <si>
+    <t>xiao hong</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>Delivery Staff</t>
+  </si>
+  <si>
     <t>cong</t>
   </si>
   <si>
@@ -43,46 +52,16 @@
     <t>Managing Staff</t>
   </si>
   <si>
-    <t>kaddhar</t>
-  </si>
-  <si>
-    <t>Anjing</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>daniel</t>
-  </si>
-  <si>
-    <t>anjing</t>
-  </si>
-  <si>
-    <t>kepong</t>
-  </si>
-  <si>
-    <t>29999</t>
+    <t>mervyn</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>Delivery Staff</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>Front Desk Staff</t>
-  </si>
-  <si>
-    <t>Charlotte</t>
-  </si>
-  <si>
-    <t>charlotte Washington</t>
-  </si>
-  <si>
-    <t>0123221256</t>
+    <t>Adelle</t>
+  </si>
+  <si>
+    <t>cong123</t>
   </si>
 </sst>
 </file>
@@ -158,30 +137,30 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -192,64 +171,115 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove email and export to excel features
</commit_message>
<xml_diff>
--- a/UserReport.xlsx
+++ b/UserReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Username</t>
   </si>
@@ -28,40 +28,133 @@
     <t>Role</t>
   </si>
   <si>
-    <t>xiao hong</t>
+    <t>Waihan</t>
+  </si>
+  <si>
+    <t>liew wai han</t>
+  </si>
+  <si>
+    <t>jade hill</t>
+  </si>
+  <si>
+    <t>01234444432</t>
+  </si>
+  <si>
+    <t>Delivery Staff</t>
+  </si>
+  <si>
+    <t>Mentos</t>
+  </si>
+  <si>
+    <t>Mentos Chill</t>
+  </si>
+  <si>
+    <t>Jalan Puteri bin Abu</t>
+  </si>
+  <si>
+    <t>0123323123212</t>
+  </si>
+  <si>
+    <t>Front Desk Staff</t>
+  </si>
+  <si>
+    <t>Donnie</t>
+  </si>
+  <si>
+    <t>Donne Ng</t>
+  </si>
+  <si>
+    <t>KLCC</t>
+  </si>
+  <si>
+    <t>012233333</t>
+  </si>
+  <si>
+    <t>cong</t>
+  </si>
+  <si>
+    <t>law wei cong</t>
+  </si>
+  <si>
+    <t>kunji</t>
+  </si>
+  <si>
+    <t>6969</t>
+  </si>
+  <si>
+    <t>Managing Staff</t>
+  </si>
+  <si>
+    <t>mervyn</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
   <si>
     <t>1234</t>
   </si>
   <si>
-    <t>Delivery Staff</t>
-  </si>
-  <si>
-    <t>cong</t>
-  </si>
-  <si>
-    <t>law wei cong</t>
-  </si>
-  <si>
-    <t>puj</t>
-  </si>
-  <si>
-    <t>6969</t>
-  </si>
-  <si>
-    <t>Managing Staff</t>
-  </si>
-  <si>
-    <t>mervyn</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Adelle</t>
-  </si>
-  <si>
-    <t>cong123</t>
+    <t>testing account</t>
+  </si>
+  <si>
+    <t>0183604709</t>
+  </si>
+  <si>
+    <t>mervyn00</t>
+  </si>
+  <si>
+    <t>testing done mervyn</t>
+  </si>
+  <si>
+    <t>haha</t>
+  </si>
+  <si>
+    <t>Tions1977</t>
+  </si>
+  <si>
+    <t>Adi�Puteri�Jebat</t>
+  </si>
+  <si>
+    <t>No. 40 Jalan 20/14</t>
+  </si>
+  <si>
+    <t>03-7955-2321</t>
+  </si>
+  <si>
+    <t>Aging1996</t>
+  </si>
+  <si>
+    <t>Sari�binti�Perang</t>
+  </si>
+  <si>
+    <t>NO 28-1 JALAN BANGSAR UTAMA 1 BANGSAR UTAMA</t>
+  </si>
+  <si>
+    <t>603 2282 3440</t>
+  </si>
+  <si>
+    <t>Hisabought69</t>
+  </si>
+  <si>
+    <t>Minah�bin�Cahaya</t>
+  </si>
+  <si>
+    <t>45 Jalan Raja Haroun</t>
+  </si>
+  <si>
+    <t>03-8736-4788</t>
+  </si>
+  <si>
+    <t>Hatheyn</t>
+  </si>
+  <si>
+    <t>Hapsah�bin�Bongsu</t>
+  </si>
+  <si>
+    <t>43-A Jalan SS15/4C</t>
+  </si>
+  <si>
+    <t>03-5634-3770</t>
   </si>
 </sst>
 </file>
@@ -137,149 +230,183 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
         <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>